<commit_message>
add  syntax for accessing specific rows on Operation's Sheets
</commit_message>
<xml_diff>
--- a/dataset/models/input/Component Curves AZA.xlsx
+++ b/dataset/models/input/Component Curves AZA.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="90">
   <si>
     <t>DataCurves</t>
   </si>
@@ -310,7 +310,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -399,27 +399,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="50">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="166" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="166" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -436,9 +433,6 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -500,28 +494,22 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="166" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
@@ -532,9 +520,6 @@
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -553,12 +538,6 @@
     </xf>
     <xf xfId="0" numFmtId="166" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="166" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -877,24 +856,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="45" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="37" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="32" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="32" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="34" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="41"/>
+      <c r="B1" s="2"/>
       <c r="C1" s="1"/>
       <c r="D1" s="3"/>
       <c r="E1" s="5"/>
@@ -908,10 +887,10 @@
       <c r="M1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="41"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
       <c r="E2" s="5"/>
@@ -925,10 +904,10 @@
       <c r="M2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1"/>
@@ -944,10 +923,10 @@
       <c r="M3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1"/>
@@ -963,10 +942,10 @@
       <c r="M4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C5" s="1"/>
@@ -982,10 +961,10 @@
       <c r="M5" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="41"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3"/>
       <c r="E6" s="5"/>
@@ -999,10 +978,10 @@
       <c r="M6" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1"/>
@@ -1018,14 +997,14 @@
       <c r="M7" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="23"/>
+      <c r="D8" s="21"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -1037,10 +1016,10 @@
       <c r="M8" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1"/>
@@ -1056,10 +1035,10 @@
       <c r="M9" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="41"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="1"/>
       <c r="D10" s="3"/>
       <c r="E10" s="5"/>
@@ -1073,10 +1052,10 @@
       <c r="M10" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
       <c r="E11" s="5"/>
@@ -1090,10 +1069,10 @@
       <c r="M11" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="41"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="1"/>
       <c r="D12" s="3"/>
       <c r="E12" s="5"/>
@@ -1108,7 +1087,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="41"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="1"/>
       <c r="D13" s="3"/>
       <c r="E13" s="5"/>
@@ -1123,7 +1102,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="41"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="1"/>
       <c r="D14" s="3"/>
       <c r="E14" s="5"/>
@@ -1138,7 +1117,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="41"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="1"/>
       <c r="D15" s="3"/>
       <c r="E15" s="5"/>
@@ -1153,7 +1132,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="41"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="1"/>
       <c r="D16" s="3"/>
       <c r="E16" s="5"/>
@@ -1168,151 +1147,151 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16" t="s">
+      <c r="C17" s="13"/>
+      <c r="D17" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="G17" s="22" t="s">
+      <c r="G17" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="H17" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="I17" s="22" t="s">
+      <c r="I17" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="J17" s="54" t="s">
+      <c r="J17" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="K17" s="54" t="s">
+      <c r="K17" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="L17" s="55" t="s">
+      <c r="L17" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="M17" s="23" t="s">
+      <c r="M17" s="21" t="s">
         <v>86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="23"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="22" t="s">
+      <c r="D18" s="25"/>
+      <c r="E18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="I18" s="22" t="s">
+      <c r="I18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="J18" s="23" t="s">
+      <c r="J18" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="K18" s="23" t="s">
+      <c r="K18" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="L18" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="M18" s="23" t="s">
+      <c r="M18" s="21" t="s">
         <v>89</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="22" t="s">
+      <c r="H19" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="22" t="s">
+      <c r="I19" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="J19" s="23" t="s">
+      <c r="J19" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="K19" s="23" t="s">
+      <c r="K19" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="L19" s="23" t="s">
+      <c r="L19" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="M19" s="23" t="s">
+      <c r="M19" s="21" t="s">
         <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="23">
+      <c r="B20" s="21">
         <v>0</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="27">
+      <c r="D20" s="25">
         <v>44713</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="20">
         <v>1</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="20">
         <v>0.7</v>
       </c>
-      <c r="G20" s="22">
+      <c r="G20" s="20">
         <v>0.04</v>
       </c>
-      <c r="H20" s="22">
+      <c r="H20" s="20">
         <v>0</v>
       </c>
-      <c r="I20" s="22">
+      <c r="I20" s="20">
         <v>0.29</v>
       </c>
-      <c r="J20" s="31">
+      <c r="J20" s="29">
         <v>25</v>
       </c>
-      <c r="K20" s="23">
+      <c r="K20" s="21">
         <v>10</v>
       </c>
-      <c r="L20" s="23">
+      <c r="L20" s="21">
         <v>10</v>
       </c>
-      <c r="M20" s="23">
+      <c r="M20" s="21">
         <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="7">
+      <c r="B21" s="2">
         <v>1</v>
       </c>
       <c r="C21" s="1"/>
@@ -1329,7 +1308,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="7">
+      <c r="B22" s="2">
         <v>2</v>
       </c>
       <c r="C22" s="1"/>
@@ -1346,7 +1325,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="7">
+      <c r="B23" s="2">
         <v>3</v>
       </c>
       <c r="C23" s="1"/>
@@ -1363,7 +1342,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="7">
+      <c r="B24" s="2">
         <v>4</v>
       </c>
       <c r="C24" s="1"/>
@@ -1380,7 +1359,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="7">
+      <c r="B25" s="2">
         <v>5</v>
       </c>
       <c r="C25" s="1"/>
@@ -1397,7 +1376,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="7">
+      <c r="B26" s="2">
         <v>6</v>
       </c>
       <c r="C26" s="1"/>
@@ -1414,7 +1393,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="7">
+      <c r="B27" s="2">
         <v>7</v>
       </c>
       <c r="C27" s="1"/>
@@ -1431,7 +1410,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="7">
+      <c r="B28" s="2">
         <v>8</v>
       </c>
       <c r="C28" s="1"/>
@@ -1448,11 +1427,11 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="7">
+      <c r="B29" s="2">
         <v>9</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="27">
+      <c r="D29" s="25">
         <v>48366</v>
       </c>
       <c r="E29" s="5"/>
@@ -1460,10 +1439,10 @@
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
-      <c r="J29" s="23">
+      <c r="J29" s="21">
         <v>39</v>
       </c>
-      <c r="K29" s="23">
+      <c r="K29" s="21">
         <v>28</v>
       </c>
       <c r="L29" s="2"/>
@@ -1471,7 +1450,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="7">
+      <c r="B30" s="2">
         <v>10</v>
       </c>
       <c r="C30" s="1"/>
@@ -1488,7 +1467,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="7">
+      <c r="B31" s="2">
         <v>11</v>
       </c>
       <c r="C31" s="1"/>
@@ -1505,7 +1484,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="7">
+      <c r="B32" s="2">
         <v>12</v>
       </c>
       <c r="C32" s="1"/>
@@ -1522,7 +1501,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="7">
+      <c r="B33" s="2">
         <v>13</v>
       </c>
       <c r="C33" s="1"/>
@@ -1539,7 +1518,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="7">
+      <c r="B34" s="2">
         <v>14</v>
       </c>
       <c r="C34" s="1"/>
@@ -1556,7 +1535,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="7">
+      <c r="B35" s="2">
         <v>15</v>
       </c>
       <c r="C35" s="1"/>
@@ -1573,7 +1552,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="7">
+      <c r="B36" s="2">
         <v>16</v>
       </c>
       <c r="C36" s="1"/>
@@ -1590,7 +1569,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="7">
+      <c r="B37" s="2">
         <v>17</v>
       </c>
       <c r="C37" s="1"/>
@@ -1607,7 +1586,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="7">
+      <c r="B38" s="2">
         <v>18</v>
       </c>
       <c r="C38" s="1"/>
@@ -1624,7 +1603,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="7">
+      <c r="B39" s="2">
         <v>19</v>
       </c>
       <c r="C39" s="1"/>
@@ -1641,7 +1620,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="7">
+      <c r="B40" s="2">
         <v>20</v>
       </c>
       <c r="C40" s="1"/>
@@ -1658,7 +1637,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="7">
+      <c r="B41" s="2">
         <v>21</v>
       </c>
       <c r="C41" s="1"/>
@@ -1689,18 +1668,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="37" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="38" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="53" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="38" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="38" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="40" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="32" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="32" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="34" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="37" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1709,7 +1688,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="34"/>
+      <c r="F1" s="5"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="4"/>
@@ -1725,7 +1704,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="34"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="4"/>
@@ -1737,13 +1716,13 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="34"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="4"/>
@@ -1755,13 +1734,13 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="34"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="4"/>
@@ -1773,13 +1752,13 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="3"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="34"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
@@ -1791,13 +1770,13 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="3"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="34"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
@@ -1809,13 +1788,13 @@
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="34"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
@@ -1827,13 +1806,13 @@
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="34"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
@@ -1845,13 +1824,13 @@
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="34"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="4"/>
@@ -1867,7 +1846,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="34"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="4"/>
@@ -1879,11 +1858,11 @@
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="34"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="4"/>
@@ -1899,7 +1878,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="3"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="34"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="4"/>
@@ -1913,7 +1892,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="3"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="34"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="4"/>
@@ -1927,7 +1906,7 @@
       <c r="C14" s="1"/>
       <c r="D14" s="3"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="34"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="4"/>
@@ -1941,7 +1920,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="3"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="34"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="4"/>
@@ -1955,7 +1934,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="3"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="34"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="4"/>
@@ -1965,135 +1944,135 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1"/>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16" t="s">
+      <c r="C17" s="13"/>
+      <c r="D17" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="I17" s="17" t="s">
+      <c r="I17" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="K17" s="50" t="s">
+      <c r="K17" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="L17" s="19" t="s">
+      <c r="L17" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="23" t="s">
+      <c r="E18" s="19"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="K18" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="L18" s="51" t="s">
+      <c r="L18" s="46" t="s">
         <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="18" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="23" t="s">
+      <c r="H19" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="21" t="s">
+      <c r="I19" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="J19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K19" s="10" t="s">
+      <c r="K19" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="L19" s="51" t="s">
+      <c r="L19" s="46" t="s">
         <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1"/>
-      <c r="B20" s="7">
+      <c r="B20" s="2">
         <v>0</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="27">
+      <c r="D20" s="25">
         <v>44713</v>
       </c>
-      <c r="E20" s="28">
+      <c r="E20" s="26">
         <v>40</v>
       </c>
-      <c r="F20" s="28">
+      <c r="F20" s="26">
         <v>8</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G20" s="28">
         <v>8</v>
       </c>
-      <c r="H20" s="31">
+      <c r="H20" s="29">
         <v>10</v>
       </c>
-      <c r="I20" s="28">
+      <c r="I20" s="26">
         <v>5</v>
       </c>
-      <c r="J20" s="30">
+      <c r="J20" s="28">
         <v>4</v>
       </c>
-      <c r="K20" s="13">
+      <c r="K20" s="4">
         <v>1.3</v>
       </c>
-      <c r="L20" s="52">
+      <c r="L20" s="6">
         <v>0.8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1"/>
-      <c r="B21" s="7">
+      <c r="B21" s="2">
         <f>1+B20</f>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="3"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="34"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="4"/>
@@ -2103,13 +2082,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1"/>
-      <c r="B22" s="7">
+      <c r="B22" s="2">
         <f>1+B21</f>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="3"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="34"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="4"/>
@@ -2119,13 +2098,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1"/>
-      <c r="B23" s="7">
+      <c r="B23" s="2">
         <f>1+B22</f>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="3"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="34"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="4"/>
@@ -2135,13 +2114,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1"/>
-      <c r="B24" s="7">
+      <c r="B24" s="2">
         <f>1+B23</f>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="3"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="34"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="4"/>
@@ -2151,13 +2130,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1"/>
-      <c r="B25" s="7">
+      <c r="B25" s="2">
         <f>1+B24</f>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="3"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="34"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="4"/>
@@ -2167,13 +2146,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1"/>
-      <c r="B26" s="7">
+      <c r="B26" s="2">
         <f>1+B25</f>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="34"/>
+      <c r="F26" s="5"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="4"/>
@@ -2183,13 +2162,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1"/>
-      <c r="B27" s="7">
+      <c r="B27" s="2">
         <f>1+B26</f>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="34"/>
+      <c r="F27" s="5"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="4"/>
@@ -2199,13 +2178,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="1"/>
-      <c r="B28" s="7">
+      <c r="B28" s="2">
         <f>1+B27</f>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="3"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="34"/>
+      <c r="F28" s="5"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="4"/>
@@ -2215,31 +2194,31 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="1"/>
-      <c r="B29" s="7">
+      <c r="B29" s="2">
         <f>1+B28</f>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="27">
+      <c r="D29" s="25">
         <v>48366</v>
       </c>
-      <c r="E29" s="28"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="30"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="28"/>
       <c r="K29" s="4"/>
       <c r="L29" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="1"/>
-      <c r="B30" s="7">
+      <c r="B30" s="2">
         <f>1+B29</f>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="3"/>
       <c r="E30" s="4"/>
-      <c r="F30" s="34"/>
+      <c r="F30" s="5"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="4"/>
@@ -2249,13 +2228,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="1"/>
-      <c r="B31" s="7">
+      <c r="B31" s="2">
         <f>1+B30</f>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="3"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="34"/>
+      <c r="F31" s="5"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="4"/>
@@ -2265,13 +2244,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="1"/>
-      <c r="B32" s="7">
+      <c r="B32" s="2">
         <f>1+B31</f>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="3"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="34"/>
+      <c r="F32" s="5"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="4"/>
@@ -2281,13 +2260,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="1"/>
-      <c r="B33" s="7">
+      <c r="B33" s="2">
         <f>1+B32</f>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="3"/>
       <c r="E33" s="4"/>
-      <c r="F33" s="34"/>
+      <c r="F33" s="5"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="4"/>
@@ -2297,13 +2276,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="1"/>
-      <c r="B34" s="7">
+      <c r="B34" s="2">
         <f>1+B33</f>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="3"/>
       <c r="E34" s="4"/>
-      <c r="F34" s="34"/>
+      <c r="F34" s="5"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="4"/>
@@ -2313,13 +2292,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="1"/>
-      <c r="B35" s="7">
+      <c r="B35" s="2">
         <f>1+B34</f>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="3"/>
       <c r="E35" s="4"/>
-      <c r="F35" s="34"/>
+      <c r="F35" s="5"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="4"/>
@@ -2329,13 +2308,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="1"/>
-      <c r="B36" s="7">
+      <c r="B36" s="2">
         <f>1+B35</f>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="3"/>
       <c r="E36" s="4"/>
-      <c r="F36" s="34"/>
+      <c r="F36" s="5"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="4"/>
@@ -2345,13 +2324,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="7">
+      <c r="B37" s="2">
         <f>1+B36</f>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="3"/>
       <c r="E37" s="4"/>
-      <c r="F37" s="34"/>
+      <c r="F37" s="5"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="4"/>
@@ -2361,13 +2340,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="7">
+      <c r="B38" s="2">
         <f>1+B37</f>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="3"/>
       <c r="E38" s="4"/>
-      <c r="F38" s="34"/>
+      <c r="F38" s="5"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="4"/>
@@ -2377,13 +2356,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="7">
+      <c r="B39" s="2">
         <f>1+B38</f>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="3"/>
       <c r="E39" s="4"/>
-      <c r="F39" s="34"/>
+      <c r="F39" s="5"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="4"/>
@@ -2393,13 +2372,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="7">
+      <c r="B40" s="2">
         <f>1+B39</f>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="3"/>
       <c r="E40" s="4"/>
-      <c r="F40" s="34"/>
+      <c r="F40" s="5"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="4"/>
@@ -2409,13 +2388,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="7">
+      <c r="B41" s="2">
         <f>1+B40</f>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="3"/>
       <c r="E41" s="4"/>
-      <c r="F41" s="34"/>
+      <c r="F41" s="5"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="4"/>
@@ -2429,7 +2408,7 @@
       <c r="C42" s="1"/>
       <c r="D42" s="3"/>
       <c r="E42" s="4"/>
-      <c r="F42" s="34"/>
+      <c r="F42" s="5"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="4"/>
@@ -2453,19 +2432,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="45" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="37" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="36" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="36" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="39" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="32" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="33" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="32" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="34" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="33" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="33" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="36" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="41"/>
+      <c r="B1" s="2"/>
       <c r="C1" s="1"/>
       <c r="D1" s="3"/>
       <c r="E1" s="2"/>
@@ -2477,7 +2456,7 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="41"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
@@ -2489,7 +2468,7 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1"/>
@@ -2503,7 +2482,7 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1"/>
@@ -2517,7 +2496,7 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C5" s="1"/>
@@ -2531,7 +2510,7 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C6" s="1"/>
@@ -2545,7 +2524,7 @@
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1"/>
@@ -2559,7 +2538,7 @@
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1"/>
@@ -2573,7 +2552,7 @@
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1"/>
@@ -2587,7 +2566,7 @@
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="41"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="1"/>
       <c r="D10" s="3"/>
       <c r="E10" s="2"/>
@@ -2599,7 +2578,7 @@
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
@@ -2611,7 +2590,7 @@
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="41"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="1"/>
       <c r="D12" s="3"/>
       <c r="E12" s="2"/>
@@ -2621,7 +2600,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="41"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="1"/>
       <c r="D13" s="3"/>
       <c r="E13" s="2"/>
@@ -2631,7 +2610,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="41"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="1"/>
       <c r="D14" s="3"/>
       <c r="E14" s="2"/>
@@ -2641,7 +2620,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="41"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="1"/>
       <c r="D15" s="3"/>
       <c r="E15" s="2"/>
@@ -2651,7 +2630,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="41"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="1"/>
       <c r="D16" s="3"/>
       <c r="E16" s="2"/>
@@ -2661,91 +2640,91 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16" t="s">
+      <c r="C17" s="13"/>
+      <c r="D17" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="26" t="s">
+      <c r="G17" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="H17" s="26" t="s">
+      <c r="H17" s="24" t="s">
         <v>73</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="41"/>
+      <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="26" t="s">
+      <c r="H18" s="24" t="s">
         <v>38</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="26" t="s">
+      <c r="H19" s="24" t="s">
         <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="7">
+      <c r="B20" s="2">
         <v>0</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="27">
+      <c r="D20" s="25">
         <v>44713</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="28">
         <v>30</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="21">
         <v>10</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="5">
         <v>0.75</v>
       </c>
-      <c r="H20" s="34">
+      <c r="H20" s="5">
         <v>0.55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="7">
+      <c r="B21" s="2">
         <f>1+B20</f>
       </c>
       <c r="C21" s="1"/>
@@ -2757,7 +2736,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="7">
+      <c r="B22" s="2">
         <f>1+B21</f>
       </c>
       <c r="C22" s="1"/>
@@ -2769,7 +2748,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="7">
+      <c r="B23" s="2">
         <f>1+B22</f>
       </c>
       <c r="C23" s="1"/>
@@ -2781,7 +2760,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="7">
+      <c r="B24" s="2">
         <f>1+B23</f>
       </c>
       <c r="C24" s="1"/>
@@ -2793,7 +2772,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="7">
+      <c r="B25" s="2">
         <f>1+B24</f>
       </c>
       <c r="C25" s="1"/>
@@ -2805,7 +2784,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="7">
+      <c r="B26" s="2">
         <f>1+B25</f>
       </c>
       <c r="C26" s="1"/>
@@ -2817,7 +2796,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="7">
+      <c r="B27" s="2">
         <f>1+B26</f>
       </c>
       <c r="C27" s="1"/>
@@ -2829,7 +2808,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="7">
+      <c r="B28" s="2">
         <f>1+B27</f>
       </c>
       <c r="C28" s="1"/>
@@ -2841,21 +2820,21 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="7">
+      <c r="B29" s="2">
         <f>1+B28</f>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="27">
+      <c r="D29" s="25">
         <v>48366</v>
       </c>
-      <c r="E29" s="30"/>
+      <c r="E29" s="28"/>
       <c r="F29" s="2"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="7">
+      <c r="B30" s="2">
         <f>1+B29</f>
       </c>
       <c r="C30" s="1"/>
@@ -2867,7 +2846,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="7">
+      <c r="B31" s="2">
         <f>1+B30</f>
       </c>
       <c r="C31" s="1"/>
@@ -2879,7 +2858,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="7">
+      <c r="B32" s="2">
         <f>1+B31</f>
       </c>
       <c r="C32" s="1"/>
@@ -2891,7 +2870,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="7">
+      <c r="B33" s="2">
         <f>1+B32</f>
       </c>
       <c r="C33" s="1"/>
@@ -2903,7 +2882,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="7">
+      <c r="B34" s="2">
         <f>1+B33</f>
       </c>
       <c r="C34" s="1"/>
@@ -2915,7 +2894,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="7">
+      <c r="B35" s="2">
         <f>1+B34</f>
       </c>
       <c r="C35" s="1"/>
@@ -2927,7 +2906,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="7">
+      <c r="B36" s="2">
         <f>1+B35</f>
       </c>
       <c r="C36" s="1"/>
@@ -2939,7 +2918,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="7">
+      <c r="B37" s="2">
         <f>1+B36</f>
       </c>
       <c r="C37" s="1"/>
@@ -2951,7 +2930,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="7">
+      <c r="B38" s="2">
         <f>1+B37</f>
       </c>
       <c r="C38" s="1"/>
@@ -2963,7 +2942,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="7">
+      <c r="B39" s="2">
         <f>1+B38</f>
       </c>
       <c r="C39" s="1"/>
@@ -2975,7 +2954,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="7">
+      <c r="B40" s="2">
         <f>1+B39</f>
       </c>
       <c r="C40" s="1"/>
@@ -2987,7 +2966,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="7">
+      <c r="B41" s="2">
         <f>1+B40</f>
       </c>
       <c r="C41" s="1"/>
@@ -3013,24 +2992,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="37" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="32" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="32" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="34" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="1"/>
@@ -3047,8 +3026,8 @@
       <c r="N1" s="5"/>
       <c r="O1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="46" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
@@ -3066,11 +3045,11 @@
       <c r="N2" s="5"/>
       <c r="O2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="46" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1"/>
@@ -3087,11 +3066,11 @@
       <c r="N3" s="5"/>
       <c r="O3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="46" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1"/>
@@ -3108,11 +3087,11 @@
       <c r="N4" s="5"/>
       <c r="O4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="46" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1"/>
@@ -3129,11 +3108,11 @@
       <c r="N5" s="5"/>
       <c r="O5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="46" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C6" s="1"/>
@@ -3150,11 +3129,11 @@
       <c r="N6" s="5"/>
       <c r="O6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="46" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1"/>
@@ -3171,15 +3150,15 @@
       <c r="N7" s="5"/>
       <c r="O7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="46" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="7"/>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3192,11 +3171,11 @@
       <c r="N8" s="5"/>
       <c r="O8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="46" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1"/>
@@ -3213,8 +3192,8 @@
       <c r="N9" s="5"/>
       <c r="O9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
-      <c r="A10" s="46" t="s">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="41" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="2"/>
@@ -3232,11 +3211,11 @@
       <c r="N10" s="5"/>
       <c r="O10" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="46" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
@@ -3251,8 +3230,8 @@
       <c r="N11" s="5"/>
       <c r="O11" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
-      <c r="A12" s="46" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="41" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="2"/>
@@ -3270,7 +3249,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
@@ -3287,7 +3266,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
@@ -3304,7 +3283,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
@@ -3321,7 +3300,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
@@ -3335,166 +3314,166 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
-      <c r="N16" s="47"/>
+      <c r="N16" s="42"/>
       <c r="O16" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1"/>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16" t="s">
+      <c r="C17" s="13"/>
+      <c r="D17" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="I17" s="47" t="s">
+      <c r="I17" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="J17" s="48" t="s">
+      <c r="J17" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="K17" s="47" t="s">
+      <c r="K17" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="L17" s="47" t="s">
+      <c r="L17" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="M17" s="49" t="s">
+      <c r="M17" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="N17" s="47" t="s">
+      <c r="N17" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="O17" s="8" t="s">
+      <c r="O17" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
-      <c r="A18" s="20" t="s">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="23"/>
-      <c r="H18" s="34"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="2"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
-      <c r="N18" s="26" t="s">
+      <c r="N18" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="O18" s="8" t="s">
+      <c r="O18" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
-      <c r="A19" s="20" t="s">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="18" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="26" t="s">
+      <c r="H19" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="26" t="s">
+      <c r="I19" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="K19" s="26" t="s">
+      <c r="K19" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="L19" s="26" t="s">
+      <c r="L19" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="M19" s="26" t="s">
+      <c r="M19" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="N19" s="26" t="s">
+      <c r="N19" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="O19" s="8" t="s">
+      <c r="O19" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1"/>
-      <c r="B20" s="7">
+      <c r="B20" s="2">
         <v>0</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="27">
+      <c r="D20" s="25">
         <v>44713</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="28">
         <v>12</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="21">
         <v>10</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="2">
         <v>10</v>
       </c>
-      <c r="H20" s="34">
+      <c r="H20" s="5">
         <v>0.45</v>
       </c>
-      <c r="I20" s="34">
+      <c r="I20" s="5">
         <v>0.04</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="2">
         <v>5</v>
       </c>
-      <c r="K20" s="34">
+      <c r="K20" s="5">
         <v>0.03</v>
       </c>
-      <c r="L20" s="34">
+      <c r="L20" s="5">
         <v>0.02</v>
       </c>
-      <c r="M20" s="34">
+      <c r="M20" s="5">
         <v>0.01</v>
       </c>
-      <c r="N20" s="34">
+      <c r="N20" s="5">
         <v>0.01</v>
       </c>
-      <c r="O20" s="7">
+      <c r="O20" s="2">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1"/>
-      <c r="B21" s="7">
+      <c r="B21" s="2">
         <v>1</v>
       </c>
       <c r="C21" s="1"/>
@@ -3511,9 +3490,9 @@
       <c r="N21" s="5"/>
       <c r="O21" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1"/>
-      <c r="B22" s="7">
+      <c r="B22" s="2">
         <v>2</v>
       </c>
       <c r="C22" s="1"/>
@@ -3530,9 +3509,9 @@
       <c r="N22" s="5"/>
       <c r="O22" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1"/>
-      <c r="B23" s="7">
+      <c r="B23" s="2">
         <v>3</v>
       </c>
       <c r="C23" s="1"/>
@@ -3549,9 +3528,9 @@
       <c r="N23" s="5"/>
       <c r="O23" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1"/>
-      <c r="B24" s="7">
+      <c r="B24" s="2">
         <v>4</v>
       </c>
       <c r="C24" s="1"/>
@@ -3568,16 +3547,16 @@
       <c r="N24" s="5"/>
       <c r="O24" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1"/>
-      <c r="B25" s="7">
+      <c r="B25" s="2">
         <v>5</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="3"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="7">
+      <c r="G25" s="2">
         <v>15</v>
       </c>
       <c r="H25" s="5"/>
@@ -3589,9 +3568,9 @@
       <c r="N25" s="5"/>
       <c r="O25" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1"/>
-      <c r="B26" s="7">
+      <c r="B26" s="2">
         <v>6</v>
       </c>
       <c r="C26" s="1"/>
@@ -3610,7 +3589,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="7">
+      <c r="B27" s="2">
         <v>7</v>
       </c>
       <c r="C27" s="1"/>
@@ -3629,7 +3608,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="7">
+      <c r="B28" s="2">
         <v>8</v>
       </c>
       <c r="C28" s="1"/>
@@ -3648,14 +3627,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="7">
+      <c r="B29" s="2">
         <v>9</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="27">
+      <c r="D29" s="25">
         <v>48366</v>
       </c>
-      <c r="E29" s="30"/>
+      <c r="E29" s="28"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="5"/>
@@ -3669,7 +3648,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="7">
+      <c r="B30" s="2">
         <v>10</v>
       </c>
       <c r="C30" s="1"/>
@@ -3688,7 +3667,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="7">
+      <c r="B31" s="2">
         <v>11</v>
       </c>
       <c r="C31" s="1"/>
@@ -3707,7 +3686,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="7">
+      <c r="B32" s="2">
         <v>12</v>
       </c>
       <c r="C32" s="1"/>
@@ -3726,7 +3705,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="7">
+      <c r="B33" s="2">
         <v>13</v>
       </c>
       <c r="C33" s="1"/>
@@ -3745,7 +3724,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="7">
+      <c r="B34" s="2">
         <v>14</v>
       </c>
       <c r="C34" s="1"/>
@@ -3764,7 +3743,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="7">
+      <c r="B35" s="2">
         <v>15</v>
       </c>
       <c r="C35" s="1"/>
@@ -3783,7 +3762,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="7">
+      <c r="B36" s="2">
         <v>16</v>
       </c>
       <c r="C36" s="1"/>
@@ -3802,7 +3781,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="7">
+      <c r="B37" s="2">
         <v>17</v>
       </c>
       <c r="C37" s="1"/>
@@ -3821,7 +3800,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="7">
+      <c r="B38" s="2">
         <v>18</v>
       </c>
       <c r="C38" s="1"/>
@@ -3840,7 +3819,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="7">
+      <c r="B39" s="2">
         <v>19</v>
       </c>
       <c r="C39" s="1"/>
@@ -3859,7 +3838,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="7">
+      <c r="B40" s="2">
         <v>20</v>
       </c>
       <c r="C40" s="1"/>
@@ -3878,7 +3857,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="7">
+      <c r="B41" s="2">
         <v>21</v>
       </c>
       <c r="C41" s="1"/>
@@ -3996,24 +3975,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="45" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="37" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="40" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="40" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="32" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="32" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="34" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="37" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="37" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="37" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="32" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="32" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="32" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="41"/>
+      <c r="B1" s="2"/>
       <c r="C1" s="1"/>
       <c r="D1" s="3"/>
       <c r="E1" s="2"/>
@@ -4030,7 +4009,7 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="41"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
@@ -4047,7 +4026,7 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1"/>
@@ -4066,7 +4045,7 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1"/>
@@ -4085,7 +4064,7 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C5" s="1"/>
@@ -4093,18 +4072,18 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="10"/>
+      <c r="M5" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1"/>
@@ -4112,18 +4091,18 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="10"/>
+      <c r="M6" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1"/>
@@ -4142,7 +4121,7 @@
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1"/>
@@ -4161,7 +4140,7 @@
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1"/>
@@ -4180,7 +4159,7 @@
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="41"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="1"/>
       <c r="D10" s="3"/>
       <c r="E10" s="2"/>
@@ -4197,7 +4176,7 @@
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
@@ -4214,7 +4193,7 @@
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="41"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="1"/>
       <c r="D12" s="3"/>
       <c r="E12" s="2"/>
@@ -4229,7 +4208,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="41"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="1"/>
       <c r="D13" s="3"/>
       <c r="E13" s="2"/>
@@ -4244,7 +4223,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="41"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="1"/>
       <c r="D14" s="3"/>
       <c r="E14" s="2"/>
@@ -4259,7 +4238,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="41"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="1"/>
       <c r="D15" s="3"/>
       <c r="E15" s="2"/>
@@ -4274,7 +4253,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="41"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="1"/>
       <c r="D16" s="3"/>
       <c r="E16" s="2"/>
@@ -4289,87 +4268,87 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16" t="s">
+      <c r="C17" s="13"/>
+      <c r="D17" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="17"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="41"/>
+      <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="23" t="s">
+      <c r="G18" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="24" t="s">
+      <c r="H18" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="24" t="s">
+      <c r="I18" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J18" s="24" t="s">
+      <c r="J18" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="21"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="24" t="s">
+      <c r="I19" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="J19" s="24" t="s">
+      <c r="J19" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K19" s="1"/>
@@ -4378,38 +4357,38 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="7">
+      <c r="B20" s="2">
         <v>0</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="27">
+      <c r="D20" s="25">
         <v>44713</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="28">
         <v>20</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F20" s="28">
         <v>20</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G20" s="28">
         <v>20</v>
       </c>
-      <c r="H20" s="32">
+      <c r="H20" s="30">
         <v>4</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="10">
         <v>4</v>
       </c>
-      <c r="J20" s="32">
+      <c r="J20" s="30">
         <v>2</v>
       </c>
-      <c r="K20" s="44"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="28"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="26"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="7">
+      <c r="B21" s="2">
         <f>1+B20</f>
       </c>
       <c r="C21" s="1"/>
@@ -4426,7 +4405,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="7">
+      <c r="B22" s="2">
         <f>1+B21</f>
       </c>
       <c r="C22" s="1"/>
@@ -4443,7 +4422,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="7">
+      <c r="B23" s="2">
         <f>1+B22</f>
       </c>
       <c r="C23" s="1"/>
@@ -4460,7 +4439,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="7">
+      <c r="B24" s="2">
         <f>1+B23</f>
       </c>
       <c r="C24" s="1"/>
@@ -4477,7 +4456,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="7">
+      <c r="B25" s="2">
         <f>1+B24</f>
       </c>
       <c r="C25" s="1"/>
@@ -4494,7 +4473,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="7">
+      <c r="B26" s="2">
         <f>1+B25</f>
       </c>
       <c r="C26" s="1"/>
@@ -4511,7 +4490,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="7">
+      <c r="B27" s="2">
         <f>1+B26</f>
       </c>
       <c r="C27" s="1"/>
@@ -4528,7 +4507,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="7">
+      <c r="B28" s="2">
         <f>1+B27</f>
       </c>
       <c r="C28" s="1"/>
@@ -4545,26 +4524,26 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="7">
+      <c r="B29" s="2">
         <f>1+B28</f>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="27">
+      <c r="D29" s="25">
         <v>48366</v>
       </c>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="26"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="7">
+      <c r="B30" s="2">
         <f>1+B29</f>
       </c>
       <c r="C30" s="1"/>
@@ -4581,7 +4560,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="7">
+      <c r="B31" s="2">
         <f>1+B30</f>
       </c>
       <c r="C31" s="1"/>
@@ -4598,7 +4577,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="7">
+      <c r="B32" s="2">
         <f>1+B31</f>
       </c>
       <c r="C32" s="1"/>
@@ -4615,7 +4594,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="7">
+      <c r="B33" s="2">
         <f>1+B32</f>
       </c>
       <c r="C33" s="1"/>
@@ -4632,7 +4611,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="7">
+      <c r="B34" s="2">
         <f>1+B33</f>
       </c>
       <c r="C34" s="1"/>
@@ -4649,7 +4628,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="7">
+      <c r="B35" s="2">
         <f>1+B34</f>
       </c>
       <c r="C35" s="1"/>
@@ -4666,7 +4645,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="7">
+      <c r="B36" s="2">
         <f>1+B35</f>
       </c>
       <c r="C36" s="1"/>
@@ -4683,7 +4662,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="7">
+      <c r="B37" s="2">
         <f>1+B36</f>
       </c>
       <c r="C37" s="1"/>
@@ -4700,7 +4679,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="7">
+      <c r="B38" s="2">
         <f>1+B37</f>
       </c>
       <c r="C38" s="1"/>
@@ -4717,7 +4696,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="7">
+      <c r="B39" s="2">
         <f>1+B38</f>
       </c>
       <c r="C39" s="1"/>
@@ -4734,7 +4713,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="7">
+      <c r="B40" s="2">
         <f>1+B39</f>
       </c>
       <c r="C40" s="1"/>
@@ -4751,7 +4730,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="7">
+      <c r="B41" s="2">
         <f>1+B40</f>
       </c>
       <c r="C41" s="1"/>
@@ -4782,26 +4761,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="37" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="38" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="38" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="40" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="38" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="39" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="32" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="32" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="34" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="37" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="35" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="33" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="36" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -4854,7 +4833,7 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1"/>
@@ -4880,7 +4859,7 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1"/>
@@ -4906,7 +4885,7 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1"/>
@@ -4919,8 +4898,8 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="10"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="9"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
@@ -4932,7 +4911,7 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1"/>
@@ -4945,8 +4924,8 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="9"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -4958,7 +4937,7 @@
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1"/>
@@ -4984,7 +4963,7 @@
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1"/>
@@ -5006,11 +4985,11 @@
       <c r="S8" s="2"/>
       <c r="T8" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1"/>
@@ -5060,7 +5039,7 @@
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
       <c r="E11" s="4"/>
@@ -5148,7 +5127,7 @@
       <c r="S14" s="2"/>
       <c r="T14" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
@@ -5166,7 +5145,7 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
-      <c r="R15" s="13"/>
+      <c r="R15" s="4"/>
       <c r="S15" s="2"/>
       <c r="T15" s="5"/>
     </row>
@@ -5194,221 +5173,227 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16" t="s">
+      <c r="C17" s="13"/>
+      <c r="D17" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="17" t="s">
+      <c r="I17" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="K17" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="14" t="s">
+      <c r="L17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="M17" s="19" t="s">
+      <c r="M17" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="N17" s="17" t="s">
+      <c r="N17" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="O17" s="14" t="s">
+      <c r="O17" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="P17" s="14" t="s">
+      <c r="P17" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="Q17" s="14" t="s">
+      <c r="Q17" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="R17" s="14" t="s">
+      <c r="R17" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="S17" s="14" t="s">
+      <c r="S17" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="T17" s="18" t="s">
+      <c r="T17" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
-      <c r="A18" s="20" t="s">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="23" t="s">
+      <c r="G18" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="23" t="s">
+      <c r="H18" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="21" t="s">
+      <c r="I18" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="J18" s="23" t="s">
+      <c r="J18" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="K18" s="23" t="s">
+      <c r="K18" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="L18" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="M18" s="24" t="s">
+      <c r="M18" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="N18" s="25" t="s">
+      <c r="N18" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="O18" s="23" t="s">
+      <c r="O18" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="P18" s="23" t="s">
+      <c r="P18" s="21" t="s">
         <v>45</v>
       </c>
       <c r="Q18" s="2"/>
-      <c r="R18" s="8" t="s">
+      <c r="R18" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="S18" s="8" t="s">
+      <c r="S18" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="T18" s="26" t="s">
+      <c r="T18" s="24" t="s">
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
-      <c r="A19" s="20" t="s">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="18" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="23" t="s">
+      <c r="H19" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="21" t="s">
+      <c r="I19" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
+      <c r="J19" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="K19" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="L19" s="21" t="s">
+        <v>48</v>
+      </c>
       <c r="M19" s="6"/>
-      <c r="N19" s="10" t="s">
+      <c r="N19" s="9" t="s">
         <v>48</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
-      <c r="Q19" s="8" t="s">
+      <c r="Q19" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="R19" s="8" t="s">
+      <c r="R19" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="S19" s="8" t="s">
+      <c r="S19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="T19" s="26" t="s">
+      <c r="T19" s="24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1"/>
-      <c r="B20" s="7">
+      <c r="B20" s="2">
         <v>0</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="27">
+      <c r="D20" s="25">
         <v>44713</v>
       </c>
-      <c r="E20" s="28">
+      <c r="E20" s="26">
         <v>3.2</v>
       </c>
-      <c r="F20" s="29">
+      <c r="F20" s="27">
         <v>0.95</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G20" s="28">
         <v>280</v>
       </c>
-      <c r="H20" s="31">
+      <c r="H20" s="29">
         <f>G20*E20</f>
       </c>
-      <c r="I20" s="28">
+      <c r="I20" s="26">
         <v>0.2</v>
       </c>
-      <c r="J20" s="30">
+      <c r="J20" s="28">
         <v>205</v>
       </c>
-      <c r="K20" s="30">
+      <c r="K20" s="28">
         <v>174</v>
       </c>
-      <c r="L20" s="30">
+      <c r="L20" s="28">
         <v>72</v>
       </c>
-      <c r="M20" s="32">
+      <c r="M20" s="30">
         <v>10</v>
       </c>
-      <c r="N20" s="7">
+      <c r="N20" s="2">
         <v>65</v>
       </c>
-      <c r="O20" s="30">
+      <c r="O20" s="28">
         <v>1</v>
       </c>
-      <c r="P20" s="33">
+      <c r="P20" s="31">
         <v>3</v>
       </c>
-      <c r="Q20" s="7">
+      <c r="Q20" s="2">
         <v>2350</v>
       </c>
-      <c r="R20" s="13">
+      <c r="R20" s="4">
         <v>0.17</v>
       </c>
-      <c r="S20" s="13">
+      <c r="S20" s="4">
         <v>3.625</v>
       </c>
-      <c r="T20" s="34">
+      <c r="T20" s="5">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1"/>
-      <c r="B21" s="7">
+      <c r="B21" s="2">
         <f>1+B20</f>
       </c>
       <c r="C21" s="1"/>
@@ -5430,9 +5415,9 @@
       <c r="S21" s="2"/>
       <c r="T21" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1"/>
-      <c r="B22" s="7">
+      <c r="B22" s="2">
         <f>1+B21</f>
       </c>
       <c r="C22" s="1"/>
@@ -5454,9 +5439,9 @@
       <c r="S22" s="2"/>
       <c r="T22" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1"/>
-      <c r="B23" s="7">
+      <c r="B23" s="2">
         <f>1+B22</f>
       </c>
       <c r="C23" s="1"/>
@@ -5478,9 +5463,9 @@
       <c r="S23" s="2"/>
       <c r="T23" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1"/>
-      <c r="B24" s="7">
+      <c r="B24" s="2">
         <f>1+B23</f>
       </c>
       <c r="C24" s="1"/>
@@ -5502,9 +5487,9 @@
       <c r="S24" s="2"/>
       <c r="T24" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1"/>
-      <c r="B25" s="7">
+      <c r="B25" s="2">
         <f>1+B24</f>
       </c>
       <c r="C25" s="1"/>
@@ -5526,9 +5511,9 @@
       <c r="S25" s="2"/>
       <c r="T25" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1"/>
-      <c r="B26" s="7">
+      <c r="B26" s="2">
         <f>1+B25</f>
       </c>
       <c r="C26" s="1"/>
@@ -5550,13 +5535,13 @@
       <c r="S26" s="2"/>
       <c r="T26" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1"/>
-      <c r="B27" s="7">
+      <c r="B27" s="2">
         <f>1+B26</f>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="27">
+      <c r="D27" s="25">
         <v>47527</v>
       </c>
       <c r="E27" s="4"/>
@@ -5571,20 +5556,20 @@
       <c r="N27" s="4"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
-      <c r="Q27" s="7">
+      <c r="Q27" s="2">
         <v>4190</v>
       </c>
-      <c r="R27" s="7">
+      <c r="R27" s="2">
         <v>1</v>
       </c>
-      <c r="S27" s="7">
+      <c r="S27" s="2">
         <v>4</v>
       </c>
       <c r="T27" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="1"/>
-      <c r="B28" s="7">
+      <c r="B28" s="2">
         <f>1+B27</f>
       </c>
       <c r="C28" s="1"/>
@@ -5606,39 +5591,39 @@
       <c r="S28" s="2"/>
       <c r="T28" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="1"/>
-      <c r="B29" s="7">
+      <c r="B29" s="2">
         <f>1+B28</f>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="27">
+      <c r="D29" s="25">
         <v>48469</v>
       </c>
-      <c r="E29" s="28"/>
-      <c r="F29" s="29">
+      <c r="E29" s="26"/>
+      <c r="F29" s="27">
         <v>0.95</v>
       </c>
-      <c r="G29" s="30"/>
-      <c r="H29" s="31">
+      <c r="G29" s="28"/>
+      <c r="H29" s="29">
         <f>H20</f>
       </c>
-      <c r="I29" s="28">
+      <c r="I29" s="26">
         <v>0.2</v>
       </c>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="11">
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="10">
         <v>2.1</v>
       </c>
-      <c r="N29" s="28">
+      <c r="N29" s="26">
         <v>0.5</v>
       </c>
-      <c r="O29" s="30">
+      <c r="O29" s="28">
         <v>1</v>
       </c>
-      <c r="P29" s="33">
+      <c r="P29" s="31">
         <v>3</v>
       </c>
       <c r="Q29" s="2"/>
@@ -5646,9 +5631,9 @@
       <c r="S29" s="2"/>
       <c r="T29" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="1"/>
-      <c r="B30" s="7">
+      <c r="B30" s="2">
         <f>1+B29</f>
       </c>
       <c r="C30" s="1"/>
@@ -5670,9 +5655,9 @@
       <c r="S30" s="2"/>
       <c r="T30" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="1"/>
-      <c r="B31" s="7">
+      <c r="B31" s="2">
         <f>1+B30</f>
       </c>
       <c r="C31" s="1"/>
@@ -5694,9 +5679,9 @@
       <c r="S31" s="2"/>
       <c r="T31" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="1"/>
-      <c r="B32" s="7">
+      <c r="B32" s="2">
         <f>1+B31</f>
       </c>
       <c r="C32" s="1"/>
@@ -5718,9 +5703,9 @@
       <c r="S32" s="2"/>
       <c r="T32" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="1"/>
-      <c r="B33" s="7">
+      <c r="B33" s="2">
         <f>1+B32</f>
       </c>
       <c r="C33" s="1"/>
@@ -5742,9 +5727,9 @@
       <c r="S33" s="2"/>
       <c r="T33" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="1"/>
-      <c r="B34" s="7">
+      <c r="B34" s="2">
         <f>1+B33</f>
       </c>
       <c r="C34" s="1"/>
@@ -5766,9 +5751,9 @@
       <c r="S34" s="2"/>
       <c r="T34" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="1"/>
-      <c r="B35" s="7">
+      <c r="B35" s="2">
         <f>1+B34</f>
       </c>
       <c r="C35" s="1"/>
@@ -5792,7 +5777,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="7">
+      <c r="B36" s="2">
         <f>1+B35</f>
       </c>
       <c r="C36" s="1"/>
@@ -5816,7 +5801,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="7">
+      <c r="B37" s="2">
         <f>1+B36</f>
       </c>
       <c r="C37" s="1"/>
@@ -5840,7 +5825,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="7">
+      <c r="B38" s="2">
         <f>1+B37</f>
       </c>
       <c r="C38" s="1"/>
@@ -5864,7 +5849,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="7">
+      <c r="B39" s="2">
         <f>1+B38</f>
       </c>
       <c r="C39" s="1"/>
@@ -5888,7 +5873,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="7">
+      <c r="B40" s="2">
         <f>1+B39</f>
       </c>
       <c r="C40" s="1"/>
@@ -5912,7 +5897,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="7">
+      <c r="B41" s="2">
         <f>1+B40</f>
       </c>
       <c r="C41" s="1"/>

</xml_diff>

<commit_message>
add data in templates report, add HFOR Keyword Operator, fix some display issus in frontend
</commit_message>
<xml_diff>
--- a/dataset/models/input/Component Curves AZA.xlsx
+++ b/dataset/models/input/Component Curves AZA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminkauffmann/Desktop/Azasimul/azasimul/dataset/models/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0798FB-BB5C-F64E-8829-C8A86EB5D28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4567AAAF-1C2A-E647-9951-CBF200E9170F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="20900" windowHeight="13540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2560" yWindow="3080" windowWidth="23080" windowHeight="13540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="System-AZA" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="102">
   <si>
     <t>DataCurves</t>
   </si>
@@ -307,6 +307,55 @@
   </si>
   <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>Service Visits per year</t>
+  </si>
+  <si>
+    <t>BMS Service life</t>
+  </si>
+  <si>
+    <t>Cabling Service life</t>
+  </si>
+  <si>
+    <t>Inverters Service life</t>
+  </si>
+  <si>
+    <t>HVAC Service life</t>
+  </si>
+  <si>
+    <t>Racks Service life</t>
+  </si>
+  <si>
+    <t>Container Enclosure Service life</t>
+  </si>
+  <si>
+    <t>Man hours per service visit</t>
+  </si>
+  <si>
+    <t>HVAC losses</t>
+  </si>
+  <si>
+    <t>End of life</t>
+  </si>
+  <si>
+    <r>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.5</t>
+    </r>
+  </si>
+  <si>
+    <t>Per Service Visit material and travel cost</t>
   </si>
 </sst>
 </file>
@@ -318,7 +367,7 @@
     <numFmt numFmtId="165" formatCode="#,##0%"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,6 +438,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -417,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -560,6 +617,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -865,9 +927,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="L5" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -875,8 +939,18 @@
     <col min="2" max="2" width="12.5" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" style="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="12.5" style="34" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="12.5" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.83203125" style="34" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="34" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" style="34" customWidth="1"/>
+    <col min="9" max="9" width="30" style="34" customWidth="1"/>
+    <col min="10" max="11" width="12.5" style="31" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.5" style="31" customWidth="1"/>
+    <col min="13" max="13" width="12.5" style="31" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" customWidth="1"/>
+    <col min="15" max="15" width="22.1640625" customWidth="1"/>
+    <col min="16" max="16" width="53.83203125" customWidth="1"/>
+    <col min="22" max="22" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1132,7 +1206,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
         <v>18</v>
       </c>
@@ -1167,8 +1241,35 @@
       <c r="M17" s="20" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N17" t="s">
+        <v>90</v>
+      </c>
+      <c r="O17" t="s">
+        <v>97</v>
+      </c>
+      <c r="P17" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q17" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="R17" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="S17" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="T17" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="U17" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="V17" s="39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="47" t="s">
         <v>36</v>
       </c>
@@ -1201,8 +1302,36 @@
       <c r="M18" s="20" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N18" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="O18" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="P18" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q18" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="R18" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="S18" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="T18" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="U18" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="V18" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="W18" s="20"/>
+    </row>
+    <row r="19" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>47</v>
       </c>
@@ -1235,8 +1364,36 @@
       <c r="M19" s="20" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="O19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="P19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="R19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="S19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="T19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="U19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="V19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="W19" s="20"/>
+    </row>
+    <row r="20" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="20">
         <v>0</v>
       </c>
@@ -1270,8 +1427,35 @@
       <c r="M20" s="20">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N20" s="20">
+        <v>2</v>
+      </c>
+      <c r="O20" s="20">
+        <v>20</v>
+      </c>
+      <c r="P20" s="20">
+        <v>5000</v>
+      </c>
+      <c r="Q20" s="20">
+        <v>10</v>
+      </c>
+      <c r="R20" s="20">
+        <v>25</v>
+      </c>
+      <c r="S20" s="20">
+        <v>20</v>
+      </c>
+      <c r="T20" s="20">
+        <v>20</v>
+      </c>
+      <c r="U20" s="20">
+        <v>20</v>
+      </c>
+      <c r="V20" s="20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>1</v>
       </c>
@@ -1286,7 +1470,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <v>2</v>
       </c>
@@ -1301,7 +1485,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
         <v>3</v>
       </c>
@@ -1316,7 +1500,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="1">
         <v>4</v>
       </c>
@@ -1331,7 +1515,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1">
         <v>5</v>
       </c>
@@ -1346,7 +1530,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="1">
         <v>6</v>
       </c>
@@ -1361,7 +1545,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="1">
         <v>7</v>
       </c>
@@ -1376,7 +1560,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="1">
         <v>8</v>
       </c>
@@ -1391,7 +1575,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="1">
         <v>9</v>
       </c>
@@ -1412,7 +1596,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="1">
         <v>10</v>
       </c>
@@ -1427,7 +1611,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1">
         <v>11</v>
       </c>
@@ -1442,7 +1626,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="1">
         <v>12</v>
       </c>
@@ -1594,6 +1778,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1604,7 +1789,7 @@
   </sheetPr>
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2317,7 +2502,9 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2523,9 +2710,7 @@
       <c r="G17" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="H17" s="23" t="s">
-        <v>73</v>
-      </c>
+      <c r="H17" s="23"/>
     </row>
     <row r="18" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
@@ -2542,9 +2727,7 @@
       <c r="G18" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="23" t="s">
-        <v>38</v>
-      </c>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
@@ -2561,9 +2744,7 @@
       <c r="G19" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="23" t="s">
-        <v>48</v>
-      </c>
+      <c r="H19" s="23"/>
     </row>
     <row r="20" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
@@ -2581,9 +2762,7 @@
       <c r="G20" s="4">
         <v>0.75</v>
       </c>
-      <c r="H20" s="4">
-        <v>0.55000000000000004</v>
-      </c>
+      <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
@@ -2820,6 +2999,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2828,9 +3008,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="F8" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3132,7 +3314,7 @@
       <c r="N16" s="40"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
         <v>18</v>
       </c>
@@ -3173,8 +3355,14 @@
       <c r="O17" s="6" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P17" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q17" s="48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>36</v>
       </c>
@@ -3199,8 +3387,14 @@
       <c r="O18" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P18" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q18" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>47</v>
       </c>
@@ -3239,8 +3433,14 @@
       <c r="O19" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P19" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q19" s="49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>0</v>
       </c>
@@ -3280,8 +3480,14 @@
       <c r="O20" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P20" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="Q20" s="50">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>1</v>
       </c>
@@ -3298,7 +3504,7 @@
       <c r="N21" s="4"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <v>2</v>
       </c>
@@ -3315,7 +3521,7 @@
       <c r="N22" s="4"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
         <v>3</v>
       </c>
@@ -3332,7 +3538,7 @@
       <c r="N23" s="4"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="1">
         <v>4</v>
       </c>
@@ -3349,7 +3555,7 @@
       <c r="N24" s="4"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1">
         <v>5</v>
       </c>
@@ -3368,7 +3574,7 @@
       <c r="N25" s="4"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="1">
         <v>6</v>
       </c>
@@ -3385,7 +3591,7 @@
       <c r="N26" s="4"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="1">
         <v>7</v>
       </c>
@@ -3402,7 +3608,7 @@
       <c r="N27" s="4"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="1">
         <v>8</v>
       </c>
@@ -3419,7 +3625,7 @@
       <c r="N28" s="4"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="1">
         <v>9</v>
       </c>
@@ -3438,7 +3644,7 @@
       <c r="N29" s="4"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="1">
         <v>10</v>
       </c>
@@ -3455,7 +3661,7 @@
       <c r="N30" s="4"/>
       <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1">
         <v>11</v>
       </c>
@@ -3472,7 +3678,7 @@
       <c r="N31" s="4"/>
       <c r="O31" s="1"/>
     </row>
-    <row r="32" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="1">
         <v>12</v>
       </c>
@@ -3719,6 +3925,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3729,7 +3936,7 @@
   </sheetPr>
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A6" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4353,10 +4560,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T48"/>
+  <dimension ref="A1:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4743,7 +4950,7 @@
       <c r="S16" s="1"/>
       <c r="T16" s="4"/>
     </row>
-    <row r="17" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
         <v>18</v>
       </c>
@@ -4799,8 +5006,11 @@
       <c r="T17" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U17" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>36</v>
       </c>
@@ -4852,8 +5062,11 @@
       <c r="T18" s="23" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>47</v>
       </c>
@@ -4901,8 +5114,11 @@
       <c r="T19" s="23" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U19" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>0</v>
       </c>
@@ -4958,8 +5174,11 @@
       <c r="T20" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <f t="shared" ref="B21:B41" si="0">1+B20</f>
         <v>1</v>
@@ -4982,7 +5201,7 @@
       <c r="S21" s="1"/>
       <c r="T21" s="4"/>
     </row>
-    <row r="22" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -5004,8 +5223,11 @@
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="4"/>
-    </row>
-    <row r="23" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -5027,8 +5249,11 @@
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="4"/>
-    </row>
-    <row r="24" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -5050,8 +5275,11 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="4"/>
-    </row>
-    <row r="25" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -5074,7 +5302,7 @@
       <c r="S25" s="1"/>
       <c r="T25" s="4"/>
     </row>
-    <row r="26" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -5096,8 +5324,11 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="4"/>
-    </row>
-    <row r="27" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -5125,8 +5356,11 @@
         <v>4</v>
       </c>
       <c r="T27" s="4"/>
-    </row>
-    <row r="28" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U27" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -5149,7 +5383,7 @@
       <c r="S28" s="1"/>
       <c r="T28" s="4"/>
     </row>
-    <row r="29" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -5189,7 +5423,7 @@
       <c r="S29" s="1"/>
       <c r="T29" s="4"/>
     </row>
-    <row r="30" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -5212,7 +5446,7 @@
       <c r="S30" s="1"/>
       <c r="T30" s="4"/>
     </row>
-    <row r="31" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -5235,7 +5469,7 @@
       <c r="S31" s="1"/>
       <c r="T31" s="4"/>
     </row>
-    <row r="32" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="1">
         <f t="shared" si="0"/>
         <v>12</v>

</xml_diff>